<commit_message>
Edit Cases and Plan.md
</commit_message>
<xml_diff>
--- a/Check.xlsx
+++ b/Check.xlsx
@@ -9,7 +9,10 @@
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <externalReferences>
+    <externalReference r:id="rId2"/>
+  </externalReferences>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -550,16 +553,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -567,15 +561,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -597,9 +582,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -609,12 +591,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -623,18 +599,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -655,17 +619,56 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -682,6 +685,27 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Лист1"/>
+      <sheetName val="Лист1 (2)"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="2">
+          <cell r="A2">
+            <v>1</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -973,8 +997,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -989,74 +1013,74 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
-      <c r="K1" s="36"/>
-      <c r="L1" s="36"/>
-      <c r="M1" s="36"/>
-      <c r="N1" s="36"/>
-      <c r="O1" s="36"/>
-      <c r="P1" s="36"/>
-      <c r="Q1" s="36"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="23"/>
+      <c r="M1" s="23"/>
+      <c r="N1" s="23"/>
+      <c r="O1" s="23"/>
+      <c r="P1" s="23"/>
+      <c r="Q1" s="23"/>
       <c r="R1" s="1"/>
     </row>
     <row r="2" spans="1:18" ht="15.75" thickBot="1">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="25" t="s">
+      <c r="C2" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="25" t="s">
+      <c r="D2" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="25" t="s">
+      <c r="E2" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="26" t="s">
+      <c r="F2" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="G2" s="26" t="s">
+      <c r="G2" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="36"/>
-      <c r="I2" s="36"/>
-      <c r="J2" s="36"/>
-      <c r="K2" s="36"/>
-      <c r="L2" s="36"/>
-      <c r="M2" s="36"/>
-      <c r="N2" s="36"/>
-      <c r="O2" s="36"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
+      <c r="K2" s="23"/>
+      <c r="L2" s="23"/>
+      <c r="M2" s="23"/>
+      <c r="N2" s="23"/>
+      <c r="O2" s="23"/>
       <c r="P2" s="5"/>
       <c r="Q2" s="5"/>
     </row>
     <row r="3" spans="1:18">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="29" t="s">
+      <c r="C3" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="31"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="22"/>
       <c r="H3" s="6"/>
       <c r="I3" s="6"/>
       <c r="J3" s="6"/>
@@ -1070,15 +1094,15 @@
       <c r="R3" s="5"/>
     </row>
     <row r="4" spans="1:18">
-      <c r="A4" s="14"/>
-      <c r="B4" s="13"/>
-      <c r="C4" s="11" t="s">
+      <c r="A4" s="42"/>
+      <c r="B4" s="34"/>
+      <c r="C4" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="12"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="9"/>
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
       <c r="J4" s="6"/>
@@ -1092,15 +1116,15 @@
       <c r="R4" s="5"/>
     </row>
     <row r="5" spans="1:18">
-      <c r="A5" s="14"/>
-      <c r="B5" s="13"/>
-      <c r="C5" s="11" t="s">
+      <c r="A5" s="42"/>
+      <c r="B5" s="34"/>
+      <c r="C5" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="12"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="9"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
       <c r="J5" s="6"/>
@@ -1114,17 +1138,17 @@
       <c r="R5" s="5"/>
     </row>
     <row r="6" spans="1:18" ht="15.75" thickBot="1">
-      <c r="A6" s="15"/>
-      <c r="B6" s="38" t="s">
+      <c r="A6" s="43"/>
+      <c r="B6" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="16" t="s">
+      <c r="C6" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="22"/>
-      <c r="G6" s="17"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="11"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
       <c r="J6" s="6"/>
@@ -1138,42 +1162,42 @@
       <c r="R6" s="5"/>
     </row>
     <row r="7" spans="1:18" ht="27" customHeight="1">
-      <c r="A7" s="33" t="s">
+      <c r="A7" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="44" t="s">
+      <c r="B7" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="29" t="s">
+      <c r="C7" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="29"/>
-      <c r="E7" s="29"/>
-      <c r="F7" s="29"/>
-      <c r="G7" s="31"/>
-      <c r="H7" s="19"/>
-      <c r="I7" s="19"/>
-      <c r="J7" s="19"/>
-      <c r="K7" s="19"/>
-      <c r="L7" s="19"/>
-      <c r="M7" s="19"/>
-      <c r="N7" s="19"/>
-      <c r="O7" s="19"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="13"/>
+      <c r="M7" s="13"/>
+      <c r="N7" s="13"/>
+      <c r="O7" s="13"/>
       <c r="P7" s="5"/>
       <c r="Q7" s="5"/>
       <c r="R7" s="5"/>
     </row>
     <row r="8" spans="1:18">
-      <c r="A8" s="23"/>
-      <c r="B8" s="45"/>
-      <c r="C8" s="11" t="s">
+      <c r="A8" s="37"/>
+      <c r="B8" s="31"/>
+      <c r="C8" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="19"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="13"/>
       <c r="I8" s="6"/>
       <c r="J8" s="6"/>
       <c r="K8" s="6"/>
@@ -1186,16 +1210,16 @@
       <c r="R8" s="5"/>
     </row>
     <row r="9" spans="1:18">
-      <c r="A9" s="23"/>
-      <c r="B9" s="45"/>
-      <c r="C9" s="11" t="s">
+      <c r="A9" s="37"/>
+      <c r="B9" s="31"/>
+      <c r="C9" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="19"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="13"/>
       <c r="I9" s="6"/>
       <c r="J9" s="6"/>
       <c r="K9" s="6"/>
@@ -1208,16 +1232,16 @@
       <c r="R9" s="5"/>
     </row>
     <row r="10" spans="1:18" ht="30">
-      <c r="A10" s="23"/>
-      <c r="B10" s="46"/>
-      <c r="C10" s="11" t="s">
+      <c r="A10" s="37"/>
+      <c r="B10" s="32"/>
+      <c r="C10" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="19"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="13"/>
       <c r="I10" s="6"/>
       <c r="J10" s="6"/>
       <c r="K10" s="6"/>
@@ -1230,18 +1254,18 @@
       <c r="R10" s="5"/>
     </row>
     <row r="11" spans="1:18" ht="30">
-      <c r="A11" s="23"/>
-      <c r="B11" s="7" t="s">
+      <c r="A11" s="37"/>
+      <c r="B11" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="19"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="13"/>
       <c r="I11" s="6"/>
       <c r="J11" s="6"/>
       <c r="K11" s="6"/>
@@ -1254,16 +1278,16 @@
       <c r="R11" s="5"/>
     </row>
     <row r="12" spans="1:18" ht="30">
-      <c r="A12" s="23"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="11" t="s">
+      <c r="A12" s="37"/>
+      <c r="B12" s="40"/>
+      <c r="C12" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="19"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="13"/>
       <c r="I12" s="6"/>
       <c r="J12" s="6"/>
       <c r="K12" s="6"/>
@@ -1276,15 +1300,15 @@
       <c r="R12" s="5"/>
     </row>
     <row r="13" spans="1:18" ht="30">
-      <c r="A13" s="23"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="11" t="s">
+      <c r="A13" s="37"/>
+      <c r="B13" s="40"/>
+      <c r="C13" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="12"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="9"/>
       <c r="H13" s="6"/>
       <c r="I13" s="6"/>
       <c r="J13" s="6"/>
@@ -1298,17 +1322,17 @@
       <c r="R13" s="5"/>
     </row>
     <row r="14" spans="1:18" ht="30">
-      <c r="A14" s="23"/>
-      <c r="B14" s="7" t="s">
+      <c r="A14" s="37"/>
+      <c r="B14" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="C14" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="12"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="9"/>
       <c r="H14" s="6"/>
       <c r="I14" s="6"/>
       <c r="J14" s="6"/>
@@ -1322,15 +1346,15 @@
       <c r="R14" s="5"/>
     </row>
     <row r="15" spans="1:18">
-      <c r="A15" s="23"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="11" t="s">
+      <c r="A15" s="37"/>
+      <c r="B15" s="40"/>
+      <c r="C15" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="12"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="9"/>
       <c r="H15" s="6"/>
       <c r="I15" s="6"/>
       <c r="J15" s="6"/>
@@ -1344,17 +1368,17 @@
       <c r="R15" s="5"/>
     </row>
     <row r="16" spans="1:18" ht="30">
-      <c r="A16" s="23"/>
-      <c r="B16" s="7" t="s">
+      <c r="A16" s="37"/>
+      <c r="B16" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C16" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="12"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="9"/>
       <c r="H16" s="6"/>
       <c r="I16" s="6"/>
       <c r="J16" s="6"/>
@@ -1368,15 +1392,15 @@
       <c r="R16" s="5"/>
     </row>
     <row r="17" spans="1:18" ht="30">
-      <c r="A17" s="23"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="11" t="s">
+      <c r="A17" s="37"/>
+      <c r="B17" s="40"/>
+      <c r="C17" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="12"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="9"/>
       <c r="H17" s="6"/>
       <c r="I17" s="6"/>
       <c r="J17" s="6"/>
@@ -1390,15 +1414,15 @@
       <c r="R17" s="5"/>
     </row>
     <row r="18" spans="1:18">
-      <c r="A18" s="23"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="11" t="s">
+      <c r="A18" s="37"/>
+      <c r="B18" s="40"/>
+      <c r="C18" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="12"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="9"/>
       <c r="H18" s="6"/>
       <c r="I18" s="6"/>
       <c r="J18" s="6"/>
@@ -1412,15 +1436,15 @@
       <c r="R18" s="5"/>
     </row>
     <row r="19" spans="1:18">
-      <c r="A19" s="23"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="11" t="s">
+      <c r="A19" s="37"/>
+      <c r="B19" s="40"/>
+      <c r="C19" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="D19" s="11"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="12"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="9"/>
       <c r="H19" s="6"/>
       <c r="I19" s="6"/>
       <c r="J19" s="6"/>
@@ -1434,15 +1458,15 @@
       <c r="R19" s="5"/>
     </row>
     <row r="20" spans="1:18" ht="30">
-      <c r="A20" s="23"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="11" t="s">
+      <c r="A20" s="37"/>
+      <c r="B20" s="40"/>
+      <c r="C20" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="12"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="9"/>
       <c r="H20" s="6"/>
       <c r="I20" s="6"/>
       <c r="J20" s="6"/>
@@ -1456,17 +1480,20 @@
       <c r="R20" s="5"/>
     </row>
     <row r="21" spans="1:18" ht="30">
-      <c r="A21" s="23"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="11" t="s">
+      <c r="A21" s="37"/>
+      <c r="B21" s="40"/>
+      <c r="C21" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="12"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="9"/>
       <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
+      <c r="I21" s="6">
+        <f>[1]Лист1!$A$2</f>
+        <v>1</v>
+      </c>
       <c r="J21" s="6"/>
       <c r="K21" s="6"/>
       <c r="L21" s="6"/>
@@ -1478,17 +1505,17 @@
       <c r="R21" s="5"/>
     </row>
     <row r="22" spans="1:18" ht="45.75" customHeight="1">
-      <c r="A22" s="23"/>
-      <c r="B22" s="32" t="s">
+      <c r="A22" s="37"/>
+      <c r="B22" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="C22" s="11" t="s">
+      <c r="C22" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="D22" s="11"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="12"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="9"/>
       <c r="H22" s="6"/>
       <c r="I22" s="6"/>
       <c r="J22" s="6"/>
@@ -1502,15 +1529,15 @@
       <c r="R22" s="5"/>
     </row>
     <row r="23" spans="1:18">
-      <c r="A23" s="23"/>
-      <c r="B23" s="32"/>
-      <c r="C23" s="11" t="s">
+      <c r="A23" s="37"/>
+      <c r="B23" s="39"/>
+      <c r="C23" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="D23" s="11"/>
-      <c r="E23" s="11"/>
-      <c r="F23" s="11"/>
-      <c r="G23" s="12"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="9"/>
       <c r="H23" s="5"/>
       <c r="I23" s="5"/>
       <c r="J23" s="5"/>
@@ -1524,15 +1551,15 @@
       <c r="R23" s="5"/>
     </row>
     <row r="24" spans="1:18">
-      <c r="A24" s="23"/>
-      <c r="B24" s="32"/>
-      <c r="C24" s="11" t="s">
+      <c r="A24" s="37"/>
+      <c r="B24" s="39"/>
+      <c r="C24" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="D24" s="11"/>
-      <c r="E24" s="11"/>
-      <c r="F24" s="11"/>
-      <c r="G24" s="12"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="9"/>
       <c r="H24" s="5"/>
       <c r="I24" s="5"/>
       <c r="J24" s="5"/>
@@ -1546,15 +1573,15 @@
       <c r="R24" s="5"/>
     </row>
     <row r="25" spans="1:18" ht="30">
-      <c r="A25" s="23"/>
-      <c r="B25" s="32"/>
-      <c r="C25" s="11" t="s">
+      <c r="A25" s="37"/>
+      <c r="B25" s="39"/>
+      <c r="C25" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="D25" s="11"/>
-      <c r="E25" s="11"/>
-      <c r="F25" s="11"/>
-      <c r="G25" s="12"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="9"/>
       <c r="H25" s="5"/>
       <c r="I25" s="5"/>
       <c r="J25" s="5"/>
@@ -1568,15 +1595,15 @@
       <c r="R25" s="5"/>
     </row>
     <row r="26" spans="1:18" ht="30">
-      <c r="A26" s="23"/>
-      <c r="B26" s="32"/>
-      <c r="C26" s="11" t="s">
+      <c r="A26" s="37"/>
+      <c r="B26" s="39"/>
+      <c r="C26" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="D26" s="11"/>
-      <c r="E26" s="11"/>
-      <c r="F26" s="11"/>
-      <c r="G26" s="12"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="9"/>
       <c r="H26" s="5"/>
       <c r="I26" s="5"/>
       <c r="J26" s="5"/>
@@ -1590,9 +1617,9 @@
       <c r="R26" s="5"/>
     </row>
     <row r="27" spans="1:18" ht="30">
-      <c r="A27" s="23"/>
-      <c r="B27" s="32"/>
-      <c r="C27" s="11" t="s">
+      <c r="A27" s="37"/>
+      <c r="B27" s="39"/>
+      <c r="C27" s="8" t="s">
         <v>38</v>
       </c>
       <c r="D27" s="2"/>
@@ -1612,9 +1639,9 @@
       <c r="R27" s="5"/>
     </row>
     <row r="28" spans="1:18" ht="45">
-      <c r="A28" s="23"/>
-      <c r="B28" s="32"/>
-      <c r="C28" s="11" t="s">
+      <c r="A28" s="37"/>
+      <c r="B28" s="39"/>
+      <c r="C28" s="8" t="s">
         <v>39</v>
       </c>
       <c r="D28" s="2"/>
@@ -1634,17 +1661,17 @@
       <c r="R28" s="5"/>
     </row>
     <row r="29" spans="1:18" ht="75">
-      <c r="A29" s="23"/>
-      <c r="B29" s="37" t="s">
+      <c r="A29" s="37"/>
+      <c r="B29" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="C29" s="11" t="s">
+      <c r="C29" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="D29" s="11"/>
-      <c r="E29" s="11"/>
-      <c r="F29" s="11"/>
-      <c r="G29" s="12"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="8"/>
+      <c r="F29" s="8"/>
+      <c r="G29" s="9"/>
       <c r="H29" s="6"/>
       <c r="I29" s="6"/>
       <c r="J29" s="6"/>
@@ -1658,17 +1685,17 @@
       <c r="R29" s="5"/>
     </row>
     <row r="30" spans="1:18" ht="60">
-      <c r="A30" s="23"/>
-      <c r="B30" s="13" t="s">
+      <c r="A30" s="37"/>
+      <c r="B30" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="C30" s="11" t="s">
+      <c r="C30" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="D30" s="11"/>
-      <c r="E30" s="11"/>
-      <c r="F30" s="11"/>
-      <c r="G30" s="12"/>
+      <c r="D30" s="8"/>
+      <c r="E30" s="8"/>
+      <c r="F30" s="8"/>
+      <c r="G30" s="9"/>
       <c r="H30" s="6"/>
       <c r="I30" s="6"/>
       <c r="J30" s="6"/>
@@ -1682,15 +1709,15 @@
       <c r="R30" s="5"/>
     </row>
     <row r="31" spans="1:18" ht="45.75" thickBot="1">
-      <c r="A31" s="34"/>
+      <c r="A31" s="38"/>
       <c r="B31" s="35"/>
-      <c r="C31" s="16" t="s">
+      <c r="C31" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="D31" s="16"/>
-      <c r="E31" s="16"/>
-      <c r="F31" s="16"/>
-      <c r="G31" s="17"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="10"/>
+      <c r="F31" s="10"/>
+      <c r="G31" s="11"/>
       <c r="H31" s="6"/>
       <c r="I31" s="6"/>
       <c r="J31" s="6"/>
@@ -1704,19 +1731,19 @@
       <c r="R31" s="5"/>
     </row>
     <row r="32" spans="1:18" ht="75.75" thickBot="1">
-      <c r="A32" s="39" t="s">
+      <c r="A32" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="B32" s="40" t="s">
+      <c r="B32" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="C32" s="41" t="s">
+      <c r="C32" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="D32" s="41"/>
-      <c r="E32" s="41"/>
-      <c r="F32" s="41"/>
-      <c r="G32" s="42"/>
+      <c r="D32" s="28"/>
+      <c r="E32" s="28"/>
+      <c r="F32" s="28"/>
+      <c r="G32" s="29"/>
       <c r="H32" s="6"/>
       <c r="I32" s="6"/>
       <c r="J32" s="6"/>
@@ -1733,16 +1760,16 @@
       <c r="A33" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B33" s="8" t="s">
+      <c r="B33" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="C33" s="29" t="s">
+      <c r="C33" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="D33" s="29"/>
-      <c r="E33" s="29"/>
-      <c r="F33" s="29"/>
-      <c r="G33" s="31"/>
+      <c r="D33" s="20"/>
+      <c r="E33" s="20"/>
+      <c r="F33" s="20"/>
+      <c r="G33" s="22"/>
       <c r="H33" s="6"/>
       <c r="I33" s="6"/>
       <c r="J33" s="6"/>
@@ -1756,227 +1783,227 @@
       <c r="R33" s="5"/>
     </row>
     <row r="34" spans="1:18">
-      <c r="A34" s="18"/>
-      <c r="B34" s="18"/>
-      <c r="C34" s="18"/>
-      <c r="D34" s="18"/>
-      <c r="E34" s="18"/>
-      <c r="F34" s="18"/>
-      <c r="G34" s="18"/>
-      <c r="H34" s="43"/>
-      <c r="I34" s="43"/>
-      <c r="J34" s="43"/>
-      <c r="K34" s="43"/>
-      <c r="L34" s="43"/>
-      <c r="M34" s="43"/>
-      <c r="N34" s="43"/>
-      <c r="O34" s="43"/>
+      <c r="A34" s="12"/>
+      <c r="B34" s="12"/>
+      <c r="C34" s="12"/>
+      <c r="D34" s="12"/>
+      <c r="E34" s="12"/>
+      <c r="F34" s="12"/>
+      <c r="G34" s="12"/>
+      <c r="H34" s="33"/>
+      <c r="I34" s="33"/>
+      <c r="J34" s="33"/>
+      <c r="K34" s="33"/>
+      <c r="L34" s="33"/>
+      <c r="M34" s="33"/>
+      <c r="N34" s="33"/>
+      <c r="O34" s="33"/>
       <c r="P34" s="5"/>
       <c r="Q34" s="5"/>
       <c r="R34" s="5"/>
     </row>
     <row r="35" spans="1:18">
-      <c r="A35" s="18"/>
-      <c r="B35" s="18"/>
-      <c r="C35" s="18"/>
-      <c r="D35" s="18"/>
-      <c r="E35" s="18"/>
-      <c r="F35" s="18"/>
-      <c r="G35" s="18"/>
-      <c r="H35" s="43"/>
-      <c r="I35" s="43"/>
-      <c r="J35" s="43"/>
-      <c r="K35" s="43"/>
-      <c r="L35" s="43"/>
-      <c r="M35" s="43"/>
-      <c r="N35" s="43"/>
-      <c r="O35" s="43"/>
+      <c r="A35" s="12"/>
+      <c r="B35" s="12"/>
+      <c r="C35" s="12"/>
+      <c r="D35" s="12"/>
+      <c r="E35" s="12"/>
+      <c r="F35" s="12"/>
+      <c r="G35" s="12"/>
+      <c r="H35" s="33"/>
+      <c r="I35" s="33"/>
+      <c r="J35" s="33"/>
+      <c r="K35" s="33"/>
+      <c r="L35" s="33"/>
+      <c r="M35" s="33"/>
+      <c r="N35" s="33"/>
+      <c r="O35" s="33"/>
       <c r="P35" s="5"/>
       <c r="Q35" s="5"/>
       <c r="R35" s="5"/>
     </row>
     <row r="36" spans="1:18">
-      <c r="A36" s="18"/>
-      <c r="B36" s="18"/>
-      <c r="C36" s="18"/>
-      <c r="D36" s="18"/>
-      <c r="E36" s="18"/>
-      <c r="F36" s="18"/>
-      <c r="G36" s="18"/>
-      <c r="H36" s="43"/>
-      <c r="I36" s="43"/>
-      <c r="J36" s="43"/>
-      <c r="K36" s="43"/>
-      <c r="L36" s="43"/>
-      <c r="M36" s="43"/>
-      <c r="N36" s="43"/>
-      <c r="O36" s="43"/>
+      <c r="A36" s="12"/>
+      <c r="B36" s="12"/>
+      <c r="C36" s="12"/>
+      <c r="D36" s="12"/>
+      <c r="E36" s="12"/>
+      <c r="F36" s="12"/>
+      <c r="G36" s="12"/>
+      <c r="H36" s="33"/>
+      <c r="I36" s="33"/>
+      <c r="J36" s="33"/>
+      <c r="K36" s="33"/>
+      <c r="L36" s="33"/>
+      <c r="M36" s="33"/>
+      <c r="N36" s="33"/>
+      <c r="O36" s="33"/>
       <c r="P36" s="5"/>
       <c r="Q36" s="5"/>
       <c r="R36" s="5"/>
     </row>
     <row r="37" spans="1:18">
-      <c r="A37" s="18"/>
-      <c r="B37" s="18"/>
-      <c r="C37" s="18"/>
-      <c r="D37" s="18"/>
-      <c r="E37" s="18"/>
-      <c r="F37" s="18"/>
-      <c r="G37" s="18"/>
-      <c r="H37" s="43"/>
-      <c r="I37" s="43"/>
-      <c r="J37" s="43"/>
-      <c r="K37" s="43"/>
-      <c r="L37" s="43"/>
-      <c r="M37" s="43"/>
-      <c r="N37" s="43"/>
-      <c r="O37" s="43"/>
+      <c r="A37" s="12"/>
+      <c r="B37" s="12"/>
+      <c r="C37" s="12"/>
+      <c r="D37" s="12"/>
+      <c r="E37" s="12"/>
+      <c r="F37" s="12"/>
+      <c r="G37" s="12"/>
+      <c r="H37" s="33"/>
+      <c r="I37" s="33"/>
+      <c r="J37" s="33"/>
+      <c r="K37" s="33"/>
+      <c r="L37" s="33"/>
+      <c r="M37" s="33"/>
+      <c r="N37" s="33"/>
+      <c r="O37" s="33"/>
       <c r="P37" s="5"/>
       <c r="Q37" s="5"/>
       <c r="R37" s="5"/>
     </row>
     <row r="38" spans="1:18">
-      <c r="A38" s="18"/>
-      <c r="B38" s="18"/>
-      <c r="C38" s="18"/>
-      <c r="D38" s="18"/>
-      <c r="E38" s="18"/>
-      <c r="F38" s="18"/>
-      <c r="G38" s="18"/>
+      <c r="A38" s="12"/>
+      <c r="B38" s="12"/>
+      <c r="C38" s="12"/>
+      <c r="D38" s="12"/>
+      <c r="E38" s="12"/>
+      <c r="F38" s="12"/>
+      <c r="G38" s="12"/>
     </row>
     <row r="39" spans="1:18">
-      <c r="A39" s="18"/>
-      <c r="B39" s="18"/>
-      <c r="C39" s="18"/>
-      <c r="D39" s="18"/>
-      <c r="E39" s="18"/>
-      <c r="F39" s="18"/>
-      <c r="G39" s="18"/>
+      <c r="A39" s="12"/>
+      <c r="B39" s="12"/>
+      <c r="C39" s="12"/>
+      <c r="D39" s="12"/>
+      <c r="E39" s="12"/>
+      <c r="F39" s="12"/>
+      <c r="G39" s="12"/>
     </row>
     <row r="40" spans="1:18">
-      <c r="A40" s="18"/>
-      <c r="B40" s="18"/>
-      <c r="C40" s="18"/>
-      <c r="D40" s="18"/>
-      <c r="E40" s="18"/>
-      <c r="F40" s="18"/>
-      <c r="G40" s="18"/>
+      <c r="A40" s="12"/>
+      <c r="B40" s="12"/>
+      <c r="C40" s="12"/>
+      <c r="D40" s="12"/>
+      <c r="E40" s="12"/>
+      <c r="F40" s="12"/>
+      <c r="G40" s="12"/>
     </row>
     <row r="41" spans="1:18">
-      <c r="A41" s="18"/>
-      <c r="B41" s="18"/>
-      <c r="C41" s="18"/>
-      <c r="D41" s="18"/>
-      <c r="E41" s="18"/>
-      <c r="F41" s="18"/>
-      <c r="G41" s="18"/>
+      <c r="A41" s="12"/>
+      <c r="B41" s="12"/>
+      <c r="C41" s="12"/>
+      <c r="D41" s="12"/>
+      <c r="E41" s="12"/>
+      <c r="F41" s="12"/>
+      <c r="G41" s="12"/>
     </row>
     <row r="42" spans="1:18">
-      <c r="A42" s="18"/>
-      <c r="B42" s="18"/>
-      <c r="C42" s="18"/>
-      <c r="D42" s="18"/>
-      <c r="E42" s="18"/>
-      <c r="F42" s="18"/>
-      <c r="G42" s="18"/>
+      <c r="A42" s="12"/>
+      <c r="B42" s="12"/>
+      <c r="C42" s="12"/>
+      <c r="D42" s="12"/>
+      <c r="E42" s="12"/>
+      <c r="F42" s="12"/>
+      <c r="G42" s="12"/>
     </row>
     <row r="43" spans="1:18">
-      <c r="A43" s="18"/>
-      <c r="B43" s="18"/>
-      <c r="C43" s="18"/>
-      <c r="D43" s="18"/>
-      <c r="E43" s="18"/>
-      <c r="F43" s="18"/>
-      <c r="G43" s="18"/>
+      <c r="A43" s="12"/>
+      <c r="B43" s="12"/>
+      <c r="C43" s="12"/>
+      <c r="D43" s="12"/>
+      <c r="E43" s="12"/>
+      <c r="F43" s="12"/>
+      <c r="G43" s="12"/>
     </row>
     <row r="44" spans="1:18">
-      <c r="A44" s="18"/>
-      <c r="B44" s="18"/>
-      <c r="C44" s="18"/>
-      <c r="D44" s="18"/>
-      <c r="E44" s="18"/>
-      <c r="F44" s="18"/>
-      <c r="G44" s="18"/>
+      <c r="A44" s="12"/>
+      <c r="B44" s="12"/>
+      <c r="C44" s="12"/>
+      <c r="D44" s="12"/>
+      <c r="E44" s="12"/>
+      <c r="F44" s="12"/>
+      <c r="G44" s="12"/>
     </row>
     <row r="45" spans="1:18">
-      <c r="A45" s="18"/>
-      <c r="B45" s="18"/>
-      <c r="C45" s="18"/>
-      <c r="D45" s="18"/>
-      <c r="E45" s="18"/>
-      <c r="F45" s="18"/>
-      <c r="G45" s="18"/>
+      <c r="A45" s="12"/>
+      <c r="B45" s="12"/>
+      <c r="C45" s="12"/>
+      <c r="D45" s="12"/>
+      <c r="E45" s="12"/>
+      <c r="F45" s="12"/>
+      <c r="G45" s="12"/>
     </row>
     <row r="46" spans="1:18">
-      <c r="A46" s="18"/>
-      <c r="B46" s="18"/>
-      <c r="C46" s="18"/>
-      <c r="D46" s="18"/>
-      <c r="E46" s="18"/>
-      <c r="F46" s="18"/>
-      <c r="G46" s="18"/>
+      <c r="A46" s="12"/>
+      <c r="B46" s="12"/>
+      <c r="C46" s="12"/>
+      <c r="D46" s="12"/>
+      <c r="E46" s="12"/>
+      <c r="F46" s="12"/>
+      <c r="G46" s="12"/>
     </row>
     <row r="47" spans="1:18">
-      <c r="A47" s="18"/>
-      <c r="B47" s="18"/>
-      <c r="C47" s="18"/>
-      <c r="D47" s="18"/>
-      <c r="E47" s="18"/>
-      <c r="F47" s="18"/>
-      <c r="G47" s="18"/>
+      <c r="A47" s="12"/>
+      <c r="B47" s="12"/>
+      <c r="C47" s="12"/>
+      <c r="D47" s="12"/>
+      <c r="E47" s="12"/>
+      <c r="F47" s="12"/>
+      <c r="G47" s="12"/>
     </row>
     <row r="48" spans="1:18">
-      <c r="A48" s="18"/>
-      <c r="B48" s="18"/>
-      <c r="C48" s="18"/>
-      <c r="D48" s="18"/>
-      <c r="E48" s="18"/>
-      <c r="F48" s="18"/>
-      <c r="G48" s="18"/>
+      <c r="A48" s="12"/>
+      <c r="B48" s="12"/>
+      <c r="C48" s="12"/>
+      <c r="D48" s="12"/>
+      <c r="E48" s="12"/>
+      <c r="F48" s="12"/>
+      <c r="G48" s="12"/>
     </row>
     <row r="49" spans="1:7">
-      <c r="A49" s="18"/>
-      <c r="B49" s="18"/>
-      <c r="C49" s="18"/>
-      <c r="D49" s="18"/>
-      <c r="E49" s="18"/>
-      <c r="F49" s="18"/>
-      <c r="G49" s="18"/>
+      <c r="A49" s="12"/>
+      <c r="B49" s="12"/>
+      <c r="C49" s="12"/>
+      <c r="D49" s="12"/>
+      <c r="E49" s="12"/>
+      <c r="F49" s="12"/>
+      <c r="G49" s="12"/>
     </row>
     <row r="50" spans="1:7">
-      <c r="A50" s="18"/>
-      <c r="B50" s="18"/>
-      <c r="C50" s="18"/>
-      <c r="D50" s="18"/>
-      <c r="E50" s="18"/>
-      <c r="F50" s="18"/>
-      <c r="G50" s="18"/>
+      <c r="A50" s="12"/>
+      <c r="B50" s="12"/>
+      <c r="C50" s="12"/>
+      <c r="D50" s="12"/>
+      <c r="E50" s="12"/>
+      <c r="F50" s="12"/>
+      <c r="G50" s="12"/>
     </row>
     <row r="51" spans="1:7">
-      <c r="A51" s="18"/>
-      <c r="B51" s="18"/>
-      <c r="C51" s="18"/>
-      <c r="D51" s="18"/>
-      <c r="E51" s="18"/>
-      <c r="F51" s="18"/>
-      <c r="G51" s="18"/>
+      <c r="A51" s="12"/>
+      <c r="B51" s="12"/>
+      <c r="C51" s="12"/>
+      <c r="D51" s="12"/>
+      <c r="E51" s="12"/>
+      <c r="F51" s="12"/>
+      <c r="G51" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A3:A6"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="A7:A31"/>
+    <mergeCell ref="B22:B28"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="B16:B21"/>
+    <mergeCell ref="B11:B13"/>
     <mergeCell ref="B7:B10"/>
     <mergeCell ref="H35:O35"/>
     <mergeCell ref="H36:O36"/>
     <mergeCell ref="H37:O37"/>
     <mergeCell ref="H34:O34"/>
     <mergeCell ref="B30:B31"/>
-    <mergeCell ref="A7:A31"/>
-    <mergeCell ref="B22:B28"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="B16:B21"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="A3:A6"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="B3:B5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>